<commit_message>
modern land hotspot islands
</commit_message>
<xml_diff>
--- a/Not Gplates/Land Calcu.xlsx
+++ b/Not Gplates/Land Calcu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Random stuff\WorldBuild\Gplates - Copy\Not Gplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E79ED4-F005-433C-B65D-1517743EC68C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23ABB78F-C8F8-4A7B-B0CE-C2B00FAC633A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -345,12 +345,6 @@
     <t>Pace: 100 (slow)</t>
   </si>
   <si>
-    <t>Pace: 280 (slow)</t>
-  </si>
-  <si>
-    <t>Pace: 290 (slow)</t>
-  </si>
-  <si>
     <t>Pace: 207 (slow)</t>
   </si>
   <si>
@@ -385,6 +379,12 @@
   </si>
   <si>
     <t>Pace: 378 (slow)</t>
+  </si>
+  <si>
+    <t>Pace: 280 (slow) Above Land</t>
+  </si>
+  <si>
+    <t>Pace: 290 (slow) Above Land</t>
   </si>
 </sst>
 </file>
@@ -730,7 +730,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -775,6 +775,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1059,7 +1060,7 @@
   <dimension ref="B1:Q48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="I4" sqref="I3:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,7 +1186,7 @@
       <c r="H6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="1"/>
+      <c r="I6" s="36"/>
       <c r="J6" s="6" t="s">
         <v>3</v>
       </c>
@@ -1211,7 +1212,7 @@
       <c r="H7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="1"/>
+      <c r="I7" s="36"/>
       <c r="J7" s="6" t="s">
         <v>3</v>
       </c>
@@ -1236,7 +1237,7 @@
       <c r="H8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="1"/>
+      <c r="I8" s="36"/>
       <c r="J8" s="6" t="s">
         <v>3</v>
       </c>
@@ -1271,7 +1272,7 @@
       <c r="H9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="1"/>
+      <c r="I9" s="36"/>
       <c r="J9" s="6" t="s">
         <v>3</v>
       </c>
@@ -1294,7 +1295,7 @@
       </c>
       <c r="C10" s="1">
         <f>O48</f>
-        <v>654</v>
+        <v>13837</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>3</v>
@@ -1302,7 +1303,7 @@
       <c r="H10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="1"/>
+      <c r="I10" s="36"/>
       <c r="J10" s="6" t="s">
         <v>3</v>
       </c>
@@ -1313,7 +1314,9 @@
       <c r="N10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O10" s="14"/>
+      <c r="O10" s="14">
+        <v>882</v>
+      </c>
       <c r="P10" s="17" t="s">
         <v>3</v>
       </c>
@@ -1327,7 +1330,7 @@
       </c>
       <c r="C11" s="29">
         <f>C9-C10</f>
-        <v>510063817.90978825</v>
+        <v>510050634.90978825</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>3</v>
@@ -1335,7 +1338,7 @@
       <c r="H11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="1"/>
+      <c r="I11" s="36"/>
       <c r="J11" s="6" t="s">
         <v>3</v>
       </c>
@@ -1346,7 +1349,9 @@
       <c r="N11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O11" s="14"/>
+      <c r="O11" s="14">
+        <v>363</v>
+      </c>
       <c r="P11" s="17" t="s">
         <v>3</v>
       </c>
@@ -1360,7 +1365,7 @@
       </c>
       <c r="C12" s="1">
         <f>C10*100/C9</f>
-        <v>1.2821908523667351E-4</v>
+        <v>2.7127943156266838E-3</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>49</v>
@@ -1368,7 +1373,7 @@
       <c r="H12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="1"/>
+      <c r="I12" s="36"/>
       <c r="J12" s="6" t="s">
         <v>3</v>
       </c>
@@ -1391,7 +1396,7 @@
       </c>
       <c r="C13" s="29">
         <f>C11*100/C9</f>
-        <v>99.999871780914773</v>
+        <v>99.997287205684387</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>49</v>
@@ -1399,7 +1404,7 @@
       <c r="H13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="1"/>
+      <c r="I13" s="36"/>
       <c r="J13" s="6" t="s">
         <v>3</v>
       </c>
@@ -1429,7 +1434,7 @@
       <c r="H14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="1"/>
+      <c r="I14" s="36"/>
       <c r="J14" s="6" t="s">
         <v>3</v>
       </c>
@@ -1440,7 +1445,9 @@
       <c r="N14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O14" s="14"/>
+      <c r="O14" s="14">
+        <v>5933</v>
+      </c>
       <c r="P14" s="17" t="s">
         <v>3</v>
       </c>
@@ -1484,7 +1491,7 @@
       </c>
       <c r="C16" s="8">
         <f>C12-C14</f>
-        <v>-28.999871780914763</v>
+        <v>-28.997287205684373</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>49</v>
@@ -1508,7 +1515,7 @@
         <v>3</v>
       </c>
       <c r="Q16" s="31" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="8:17" x14ac:dyDescent="0.25">
@@ -1531,7 +1538,7 @@
         <v>3</v>
       </c>
       <c r="Q17" s="31" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="8:17" x14ac:dyDescent="0.25">
@@ -1549,12 +1556,14 @@
       <c r="N18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O18" s="14"/>
+      <c r="O18" s="14">
+        <v>6005</v>
+      </c>
       <c r="P18" s="17" t="s">
         <v>3</v>
       </c>
       <c r="Q18" s="31" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="8:17" x14ac:dyDescent="0.25">
@@ -1577,7 +1586,7 @@
         <v>3</v>
       </c>
       <c r="Q19" s="31" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="8:17" x14ac:dyDescent="0.25">
@@ -1621,7 +1630,7 @@
         <v>3</v>
       </c>
       <c r="Q21" s="35" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="8:17" x14ac:dyDescent="0.25">
@@ -1688,7 +1697,7 @@
         <v>3</v>
       </c>
       <c r="Q24" s="31" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="8:17" x14ac:dyDescent="0.25">
@@ -1711,7 +1720,7 @@
         <v>3</v>
       </c>
       <c r="Q25" s="31" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="8:17" x14ac:dyDescent="0.25">
@@ -1776,7 +1785,7 @@
         <v>3</v>
       </c>
       <c r="Q28" s="31" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="8:17" x14ac:dyDescent="0.25">
@@ -1857,7 +1866,7 @@
         <v>3</v>
       </c>
       <c r="Q32" s="31" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="4:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1880,7 +1889,7 @@
         <v>3</v>
       </c>
       <c r="Q33" s="31" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="4:17" x14ac:dyDescent="0.25">
@@ -1896,7 +1905,7 @@
         <v>3</v>
       </c>
       <c r="Q34" s="31" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="4:17" x14ac:dyDescent="0.25">
@@ -1912,7 +1921,7 @@
         <v>3</v>
       </c>
       <c r="Q35" s="31" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="4:17" x14ac:dyDescent="0.25">
@@ -1928,7 +1937,7 @@
         <v>3</v>
       </c>
       <c r="Q36" s="31" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="4:17" x14ac:dyDescent="0.25">
@@ -1947,7 +1956,7 @@
         <v>3</v>
       </c>
       <c r="Q37" s="31" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="4:17" x14ac:dyDescent="0.25">
@@ -2125,7 +2134,7 @@
       </c>
       <c r="O48" s="26">
         <f>SUM(O3:O47)</f>
-        <v>654</v>
+        <v>13837</v>
       </c>
       <c r="P48" s="27" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
split, orogeny fixes, exit
</commit_message>
<xml_diff>
--- a/Not Gplates/Land Calcu.xlsx
+++ b/Not Gplates/Land Calcu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Random stuff\WorldBuild\Gplates - Copy\Not Gplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF61265-938D-49FF-B771-3525E74CEE6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87D2120-C57F-4176-A86B-E44EBACDBCE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="125">
   <si>
     <t>Name</t>
   </si>
@@ -381,9 +381,6 @@
     <t>Hotspot X12</t>
   </si>
   <si>
-    <t>Pace: 187</t>
-  </si>
-  <si>
     <t>d</t>
   </si>
   <si>
@@ -400,6 +397,18 @@
   </si>
   <si>
     <t>Continent Boscalis</t>
+  </si>
+  <si>
+    <t>Pace: 187 (slow)</t>
+  </si>
+  <si>
+    <t>ToDo</t>
+  </si>
+  <si>
+    <t>Felülvizsgálni a Hotspotokat (sárga)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We need more crust </t>
   </si>
 </sst>
 </file>
@@ -432,7 +441,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -457,6 +466,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="28">
     <border>
@@ -764,7 +779,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -828,6 +843,15 @@
     <xf numFmtId="166" fontId="0" fillId="3" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1109,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:Q48"/>
+  <dimension ref="B1:V48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1121,14 +1145,14 @@
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.42578125" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6.42578125" customWidth="1"/>
     <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="70.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1143,8 +1167,14 @@
       <c r="Q2" s="12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="S2" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="4"/>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>36</v>
       </c>
@@ -1157,14 +1187,12 @@
       <c r="H3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="3">
-        <v>502641.12520000001</v>
-      </c>
+      <c r="I3" s="3"/>
       <c r="J3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M3" s="47">
         <v>54102303.048900001</v>
@@ -1177,8 +1205,14 @@
         <v>3</v>
       </c>
       <c r="Q3" s="30"/>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="S3" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="6"/>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>37</v>
       </c>
@@ -1191,16 +1225,16 @@
       <c r="H4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="1">
-        <v>976944.91299999994</v>
-      </c>
+      <c r="I4" s="1"/>
       <c r="J4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="M4" s="47"/>
+        <v>120</v>
+      </c>
+      <c r="M4" s="47">
+        <v>55076575.485200003</v>
+      </c>
       <c r="N4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1209,13 +1243,19 @@
         <v>3</v>
       </c>
       <c r="Q4" s="30"/>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="S4" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="6"/>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C5" s="46">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>40</v>
@@ -1223,9 +1263,7 @@
       <c r="H5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="1">
-        <v>381696.79060000001</v>
-      </c>
+      <c r="I5" s="1"/>
       <c r="J5" s="6" t="s">
         <v>3</v>
       </c>
@@ -1245,8 +1283,12 @@
       <c r="Q5" s="30" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="S5" s="5"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="6"/>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="1"/>
       <c r="D6" s="6"/>
@@ -1267,14 +1309,18 @@
         <v>3</v>
       </c>
       <c r="Q6" s="30"/>
-    </row>
-    <row r="7" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S6" s="5"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="6"/>
+    </row>
+    <row r="7" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C7" s="38">
         <f>C4*(C5-50)/2</f>
-        <v>236250</v>
+        <v>26250</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>3</v>
@@ -1302,8 +1348,12 @@
       <c r="Q7" s="43" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="8" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S7" s="5"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="6"/>
+    </row>
+    <row r="8" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H8" s="5" t="s">
         <v>13</v>
       </c>
@@ -1327,8 +1377,12 @@
       <c r="Q8" s="44" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="S8" s="5"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="6"/>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>41</v>
       </c>
@@ -1362,14 +1416,18 @@
         <v>3</v>
       </c>
       <c r="Q9" s="44"/>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="S9" s="5"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="6"/>
+    </row>
+    <row r="10" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="1">
-        <f>O48</f>
-        <v>599724</v>
+      <c r="C10" s="29">
+        <f>M48</f>
+        <v>111556962.36289999</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>3</v>
@@ -1399,14 +1457,18 @@
       <c r="Q10" s="44" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="S10" s="7"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="9"/>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>43</v>
       </c>
       <c r="C11" s="29">
         <f>C9-C10</f>
-        <v>509464747.90978825</v>
+        <v>398507509.54688823</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>3</v>
@@ -1435,13 +1497,13 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C12" s="1">
         <f>C10*100/C9</f>
-        <v>0.11757807748391251</v>
+        <v>21.87114933631965</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>49</v>
@@ -1470,13 +1532,13 @@
       </c>
       <c r="Q12" s="44"/>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C13" s="29">
         <f>C11*100/C9</f>
-        <v>99.882421922516087</v>
+        <v>78.128850663680339</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>49</v>
@@ -1489,7 +1551,7 @@
         <v>3</v>
       </c>
       <c r="L13" s="39" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M13" s="50"/>
       <c r="N13" s="41" t="s">
@@ -1503,7 +1565,7 @@
       </c>
       <c r="Q13" s="44"/>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>46</v>
       </c>
@@ -1520,24 +1582,24 @@
       <c r="J14" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L14" s="39" t="s">
+      <c r="L14" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="M14" s="50"/>
-      <c r="N14" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O14" s="40">
+      <c r="M14" s="54"/>
+      <c r="N14" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="O14" s="56">
         <v>5933</v>
       </c>
-      <c r="P14" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q14" s="44" t="s">
+      <c r="P14" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q14" s="58" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>47</v>
       </c>
@@ -1569,13 +1631,13 @@
       </c>
       <c r="Q15" s="44"/>
     </row>
-    <row r="16" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>48</v>
       </c>
       <c r="C16" s="8">
         <f>C12-C14</f>
-        <v>-28.882421922516087</v>
+        <v>-7.1288506636803497</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>49</v>
@@ -1633,20 +1695,20 @@
       <c r="J18" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L18" s="39" t="s">
+      <c r="L18" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="M18" s="50"/>
-      <c r="N18" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O18" s="40">
+      <c r="M18" s="54"/>
+      <c r="N18" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="O18" s="56">
         <v>6005</v>
       </c>
-      <c r="P18" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q18" s="44" t="s">
+      <c r="P18" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q18" s="58" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1658,20 +1720,20 @@
       <c r="J19" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L19" s="39" t="s">
+      <c r="L19" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="M19" s="50"/>
-      <c r="N19" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O19" s="40">
+      <c r="M19" s="54"/>
+      <c r="N19" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="O19" s="56">
         <v>7519</v>
       </c>
-      <c r="P19" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q19" s="44" t="s">
+      <c r="P19" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q19" s="58" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1708,20 +1770,20 @@
       <c r="J21" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L21" s="45" t="s">
+      <c r="L21" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="M21" s="50"/>
-      <c r="N21" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O21" s="40">
+      <c r="M21" s="54"/>
+      <c r="N21" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="O21" s="56">
         <v>4228</v>
       </c>
-      <c r="P21" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q21" s="44" t="s">
+      <c r="P21" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q21" s="58" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1783,20 +1845,20 @@
       <c r="J24" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L24" s="39" t="s">
+      <c r="L24" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="M24" s="50"/>
-      <c r="N24" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O24" s="40">
+      <c r="M24" s="54"/>
+      <c r="N24" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="O24" s="56">
         <v>7127</v>
       </c>
-      <c r="P24" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q24" s="44" t="s">
+      <c r="P24" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q24" s="58" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1879,20 +1941,20 @@
       <c r="J28" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L28" s="39" t="s">
+      <c r="L28" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="M28" s="50"/>
-      <c r="N28" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O28" s="40">
+      <c r="M28" s="54"/>
+      <c r="N28" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="O28" s="56">
         <v>1530</v>
       </c>
-      <c r="P28" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q28" s="44" t="s">
+      <c r="P28" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q28" s="58" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1923,7 +1985,7 @@
     </row>
     <row r="30" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H30" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I30" s="1"/>
       <c r="J30" s="6" t="s">
@@ -1973,25 +2035,25 @@
       </c>
       <c r="I32" s="1">
         <f>SUM(I3:I29)</f>
-        <v>1861282.8287999998</v>
+        <v>0</v>
       </c>
       <c r="J32" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L32" s="39" t="s">
+      <c r="L32" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="M32" s="50"/>
-      <c r="N32" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O32" s="40">
+      <c r="M32" s="54"/>
+      <c r="N32" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="O32" s="56">
         <v>3583</v>
       </c>
-      <c r="P32" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q32" s="44" t="s">
+      <c r="P32" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q32" s="58" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2001,61 +2063,61 @@
       </c>
       <c r="I33" s="8">
         <f>I34-I32</f>
-        <v>-1861282.8287999998</v>
+        <v>0</v>
       </c>
       <c r="J33" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="L33" s="39" t="s">
+      <c r="L33" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="M33" s="50"/>
-      <c r="N33" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O33" s="40">
+      <c r="M33" s="54"/>
+      <c r="N33" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="O33" s="56">
         <v>643</v>
       </c>
-      <c r="P33" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q33" s="44" t="s">
+      <c r="P33" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q33" s="58" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="34" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="L34" s="39" t="s">
+      <c r="L34" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="M34" s="50"/>
-      <c r="N34" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O34" s="40">
+      <c r="M34" s="54"/>
+      <c r="N34" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="O34" s="56">
         <v>369</v>
       </c>
-      <c r="P34" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q34" s="44" t="s">
+      <c r="P34" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q34" s="58" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="35" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="L35" s="39" t="s">
+      <c r="L35" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="M35" s="50"/>
-      <c r="N35" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O35" s="40">
+      <c r="M35" s="54"/>
+      <c r="N35" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="O35" s="56">
         <v>446</v>
       </c>
-      <c r="P35" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q35" s="44" t="s">
+      <c r="P35" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q35" s="58" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2111,21 +2173,21 @@
         <v>87</v>
       </c>
       <c r="I38" s="21"/>
-      <c r="L38" s="39" t="s">
+      <c r="L38" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="M38" s="50"/>
-      <c r="N38" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O38" s="40">
+      <c r="M38" s="54"/>
+      <c r="N38" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="O38" s="56">
         <v>6852</v>
       </c>
-      <c r="P38" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q38" s="44" t="s">
-        <v>115</v>
+      <c r="P38" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q38" s="58" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="4:17" x14ac:dyDescent="0.25">
@@ -2144,7 +2206,7 @@
       </c>
       <c r="I39" s="17"/>
       <c r="L39" s="39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M39" s="50"/>
       <c r="N39" s="41" t="s">
@@ -2173,22 +2235,22 @@
         <v>89</v>
       </c>
       <c r="I40" s="24"/>
-      <c r="L40" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="M40" s="52">
+      <c r="L40" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="M40" s="50">
         <v>236250</v>
       </c>
-      <c r="N40" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O40" s="14">
+      <c r="N40" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O40" s="40">
         <v>236466</v>
       </c>
-      <c r="P40" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q40" s="30"/>
+      <c r="P40" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q40" s="44"/>
     </row>
     <row r="41" spans="4:17" x14ac:dyDescent="0.25">
       <c r="L41" s="5"/>
@@ -2280,7 +2342,7 @@
       </c>
       <c r="M48" s="48">
         <f>SUM(M3:M47)</f>
-        <v>56480386.877700001</v>
+        <v>111556962.36289999</v>
       </c>
       <c r="N48" s="26" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
hotspot island fix pt1
</commit_message>
<xml_diff>
--- a/Not Gplates/Land Calcu.xlsx
+++ b/Not Gplates/Land Calcu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Random stuff\WorldBuild\Gplates - Copy\Not Gplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87D2120-C57F-4176-A86B-E44EBACDBCE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05E5E4C-0B84-4239-9635-285F99FBFB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="126">
   <si>
     <t>Name</t>
   </si>
@@ -409,6 +409,9 @@
   </si>
   <si>
     <t xml:space="preserve">We need more crust </t>
+  </si>
+  <si>
+    <t>kellene még</t>
   </si>
 </sst>
 </file>
@@ -417,7 +420,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -779,7 +782,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -818,15 +821,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -840,18 +841,19 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1133,10 +1135,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:V48"/>
+  <dimension ref="B1:V49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+      <selection activeCell="O50" sqref="O50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,7 +1149,7 @@
     <col min="12" max="12" width="22.42578125" customWidth="1"/>
     <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6.42578125" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="70.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1194,13 +1196,16 @@
       <c r="L3" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="M3" s="47">
+      <c r="M3" s="45">
         <v>54102303.048900001</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="14"/>
+      <c r="O3" s="57">
+        <f>M3</f>
+        <v>54102303.048900001</v>
+      </c>
       <c r="P3" s="17" t="s">
         <v>3</v>
       </c>
@@ -1216,7 +1221,7 @@
       <c r="B4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="46">
+      <c r="C4" s="44">
         <v>1050</v>
       </c>
       <c r="D4" s="6" t="s">
@@ -1232,13 +1237,16 @@
       <c r="L4" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="M4" s="47">
+      <c r="M4" s="45">
         <v>55076575.485200003</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="14"/>
+      <c r="O4" s="57">
+        <f t="shared" ref="O4:O5" si="0">M4</f>
+        <v>55076575.485200003</v>
+      </c>
       <c r="P4" s="17" t="s">
         <v>3</v>
       </c>
@@ -1254,7 +1262,7 @@
       <c r="B5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="46">
+      <c r="C5" s="44">
         <v>100</v>
       </c>
       <c r="D5" s="6" t="s">
@@ -1270,13 +1278,16 @@
       <c r="L5" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="M5" s="47">
+      <c r="M5" s="45">
         <v>1861282.8287999998</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O5" s="14"/>
+      <c r="O5" s="57">
+        <f t="shared" si="0"/>
+        <v>1861282.8287999998</v>
+      </c>
       <c r="P5" s="17" t="s">
         <v>3</v>
       </c>
@@ -1300,7 +1311,7 @@
         <v>3</v>
       </c>
       <c r="L6" s="5"/>
-      <c r="M6" s="47"/>
+      <c r="M6" s="45"/>
       <c r="N6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1318,7 +1329,7 @@
       <c r="B7" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7" s="37">
         <f>C4*(C5-50)/2</f>
         <v>26250</v>
       </c>
@@ -1332,20 +1343,20 @@
       <c r="J7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L7" s="39" t="s">
+      <c r="L7" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="M7" s="50"/>
-      <c r="N7" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O7" s="40">
+      <c r="M7" s="48"/>
+      <c r="N7" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="O7" s="48">
         <v>418</v>
       </c>
-      <c r="P7" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q7" s="43" t="s">
+      <c r="P7" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="41" t="s">
         <v>95</v>
       </c>
       <c r="S7" s="5"/>
@@ -1361,20 +1372,20 @@
       <c r="J8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L8" s="39" t="s">
+      <c r="L8" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="M8" s="50"/>
-      <c r="N8" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O8" s="40">
+      <c r="M8" s="48"/>
+      <c r="N8" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="O8" s="48">
         <v>236</v>
       </c>
-      <c r="P8" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q8" s="44" t="s">
+      <c r="P8" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q8" s="42" t="s">
         <v>96</v>
       </c>
       <c r="S8" s="5"/>
@@ -1400,22 +1411,22 @@
       <c r="J9" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L9" s="39" t="s">
+      <c r="L9" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="M9" s="50">
+      <c r="M9" s="48">
         <v>26300</v>
       </c>
-      <c r="N9" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O9" s="40">
+      <c r="N9" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="O9" s="48">
         <v>26303</v>
       </c>
-      <c r="P9" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q9" s="44"/>
+      <c r="P9" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="42"/>
       <c r="S9" s="5"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
@@ -1426,8 +1437,8 @@
         <v>42</v>
       </c>
       <c r="C10" s="29">
-        <f>M48</f>
-        <v>111556962.36289999</v>
+        <f>O48</f>
+        <v>111667380.73939998</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>3</v>
@@ -1439,22 +1450,22 @@
       <c r="J10" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L10" s="39" t="s">
+      <c r="L10" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="M10" s="50">
+      <c r="M10" s="48">
         <v>1</v>
       </c>
-      <c r="N10" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O10" s="40">
+      <c r="N10" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="O10" s="48">
         <v>882</v>
       </c>
-      <c r="P10" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q10" s="44" t="s">
+      <c r="P10" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="42" t="s">
         <v>97</v>
       </c>
       <c r="S10" s="7"/>
@@ -1468,7 +1479,7 @@
       </c>
       <c r="C11" s="29">
         <f>C9-C10</f>
-        <v>398507509.54688823</v>
+        <v>398397091.17038828</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>3</v>
@@ -1480,20 +1491,20 @@
       <c r="J11" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L11" s="39" t="s">
+      <c r="L11" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="M11" s="50"/>
-      <c r="N11" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O11" s="40">
+      <c r="M11" s="48"/>
+      <c r="N11" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="O11" s="48">
         <v>363</v>
       </c>
-      <c r="P11" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q11" s="44" t="s">
+      <c r="P11" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q11" s="42" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1503,7 +1514,7 @@
       </c>
       <c r="C12" s="1">
         <f>C10*100/C9</f>
-        <v>21.87114933631965</v>
+        <v>21.892797261744956</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>49</v>
@@ -1515,22 +1526,22 @@
       <c r="J12" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L12" s="39" t="s">
+      <c r="L12" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="M12" s="50">
+      <c r="M12" s="48">
         <v>37000</v>
       </c>
-      <c r="N12" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O12" s="40">
+      <c r="N12" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="O12" s="48">
         <v>38717</v>
       </c>
-      <c r="P12" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q12" s="44"/>
+      <c r="P12" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q12" s="42"/>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
@@ -1538,7 +1549,7 @@
       </c>
       <c r="C13" s="29">
         <f>C11*100/C9</f>
-        <v>78.128850663680339</v>
+        <v>78.10720273825504</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>49</v>
@@ -1550,20 +1561,20 @@
       <c r="J13" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L13" s="39" t="s">
+      <c r="L13" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="M13" s="50"/>
-      <c r="N13" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O13" s="40">
+      <c r="M13" s="48"/>
+      <c r="N13" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="O13" s="48">
         <v>816</v>
       </c>
-      <c r="P13" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q13" s="44"/>
+      <c r="P13" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q13" s="42"/>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
@@ -1582,20 +1593,20 @@
       <c r="J14" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L14" s="53" t="s">
+      <c r="L14" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="M14" s="54"/>
-      <c r="N14" s="55" t="s">
-        <v>3</v>
-      </c>
-      <c r="O14" s="56">
-        <v>5933</v>
-      </c>
-      <c r="P14" s="57" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q14" s="58" t="s">
+      <c r="M14" s="48"/>
+      <c r="N14" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="O14" s="48">
+        <v>17074</v>
+      </c>
+      <c r="P14" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q14" s="42" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1616,20 +1627,20 @@
       <c r="J15" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L15" s="39" t="s">
+      <c r="L15" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="M15" s="50"/>
-      <c r="N15" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O15" s="40">
+      <c r="M15" s="48"/>
+      <c r="N15" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="O15" s="48">
         <v>1516</v>
       </c>
-      <c r="P15" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q15" s="44"/>
+      <c r="P15" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q15" s="42"/>
     </row>
     <row r="16" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
@@ -1637,7 +1648,7 @@
       </c>
       <c r="C16" s="8">
         <f>C12-C14</f>
-        <v>-7.1288506636803497</v>
+        <v>-7.1072027382550438</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>49</v>
@@ -1652,15 +1663,15 @@
       <c r="L16" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="M16" s="51"/>
-      <c r="N16" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="O16" s="34"/>
-      <c r="P16" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q16" s="37" t="s">
+      <c r="M16" s="49"/>
+      <c r="N16" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="O16" s="49"/>
+      <c r="P16" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q16" s="36" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1675,15 +1686,15 @@
       <c r="L17" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="M17" s="51"/>
-      <c r="N17" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="O17" s="34"/>
-      <c r="P17" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q17" s="37" t="s">
+      <c r="M17" s="49"/>
+      <c r="N17" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="O17" s="49"/>
+      <c r="P17" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q17" s="36" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1695,20 +1706,20 @@
       <c r="J18" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L18" s="53" t="s">
+      <c r="L18" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="M18" s="54"/>
-      <c r="N18" s="55" t="s">
-        <v>3</v>
-      </c>
-      <c r="O18" s="56">
-        <v>6005</v>
-      </c>
-      <c r="P18" s="57" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q18" s="58" t="s">
+      <c r="M18" s="48"/>
+      <c r="N18" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="O18" s="48">
+        <v>22359.376500000002</v>
+      </c>
+      <c r="P18" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q18" s="42" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1720,20 +1731,20 @@
       <c r="J19" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L19" s="53" t="s">
+      <c r="L19" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="M19" s="54"/>
-      <c r="N19" s="55" t="s">
-        <v>3</v>
-      </c>
-      <c r="O19" s="56">
+      <c r="M19" s="52"/>
+      <c r="N19" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="O19" s="52">
         <v>7519</v>
       </c>
-      <c r="P19" s="57" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q19" s="58" t="s">
+      <c r="P19" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q19" s="55" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1745,22 +1756,22 @@
       <c r="J20" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L20" s="45" t="s">
+      <c r="L20" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="M20" s="50">
+      <c r="M20" s="48">
         <v>34000</v>
       </c>
-      <c r="N20" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O20" s="40">
+      <c r="N20" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="O20" s="48">
         <v>34074</v>
       </c>
-      <c r="P20" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q20" s="44"/>
+      <c r="P20" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q20" s="42"/>
     </row>
     <row r="21" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H21" s="5" t="s">
@@ -1770,20 +1781,20 @@
       <c r="J21" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L21" s="59" t="s">
+      <c r="L21" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="M21" s="54"/>
-      <c r="N21" s="55" t="s">
-        <v>3</v>
-      </c>
-      <c r="O21" s="56">
+      <c r="M21" s="52"/>
+      <c r="N21" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="O21" s="52">
         <v>4228</v>
       </c>
-      <c r="P21" s="57" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q21" s="58" t="s">
+      <c r="P21" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q21" s="55" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1795,20 +1806,20 @@
       <c r="J22" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L22" s="45" t="s">
+      <c r="L22" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="M22" s="50"/>
-      <c r="N22" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O22" s="40">
+      <c r="M22" s="48"/>
+      <c r="N22" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="O22" s="48">
         <v>2307</v>
       </c>
-      <c r="P22" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q22" s="44" t="s">
+      <c r="P22" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q22" s="42" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1820,22 +1831,22 @@
       <c r="J23" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L23" s="45" t="s">
+      <c r="L23" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="M23" s="50">
+      <c r="M23" s="48">
         <v>71250</v>
       </c>
-      <c r="N23" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O23" s="40">
+      <c r="N23" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="O23" s="48">
         <v>71285</v>
       </c>
-      <c r="P23" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q23" s="44"/>
+      <c r="P23" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q23" s="42"/>
     </row>
     <row r="24" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H24" s="5" t="s">
@@ -1845,20 +1856,20 @@
       <c r="J24" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L24" s="53" t="s">
+      <c r="L24" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="M24" s="54"/>
-      <c r="N24" s="55" t="s">
-        <v>3</v>
-      </c>
-      <c r="O24" s="56">
+      <c r="M24" s="52"/>
+      <c r="N24" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="O24" s="52">
         <v>7127</v>
       </c>
-      <c r="P24" s="57" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q24" s="58" t="s">
+      <c r="P24" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q24" s="55" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1873,15 +1884,15 @@
       <c r="L25" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="M25" s="51"/>
-      <c r="N25" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="O25" s="34"/>
-      <c r="P25" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q25" s="37" t="s">
+      <c r="M25" s="49"/>
+      <c r="N25" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="O25" s="49"/>
+      <c r="P25" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q25" s="36" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1893,22 +1904,22 @@
       <c r="J26" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L26" s="39" t="s">
+      <c r="L26" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="M26" s="50">
+      <c r="M26" s="48">
         <v>12250</v>
       </c>
-      <c r="N26" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O26" s="40">
+      <c r="N26" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="O26" s="48">
         <v>13077</v>
       </c>
-      <c r="P26" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q26" s="44"/>
+      <c r="P26" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q26" s="42"/>
     </row>
     <row r="27" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H27" s="5" t="s">
@@ -1918,20 +1929,20 @@
       <c r="J27" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L27" s="39" t="s">
+      <c r="L27" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="M27" s="50"/>
-      <c r="N27" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O27" s="40">
+      <c r="M27" s="48"/>
+      <c r="N27" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="O27" s="48">
         <v>2402</v>
       </c>
-      <c r="P27" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q27" s="44"/>
+      <c r="P27" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q27" s="42"/>
     </row>
     <row r="28" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H28" s="5" t="s">
@@ -1941,20 +1952,20 @@
       <c r="J28" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L28" s="53" t="s">
+      <c r="L28" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="M28" s="54"/>
-      <c r="N28" s="55" t="s">
-        <v>3</v>
-      </c>
-      <c r="O28" s="56">
+      <c r="M28" s="52"/>
+      <c r="N28" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="O28" s="52">
         <v>1530</v>
       </c>
-      <c r="P28" s="57" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q28" s="58" t="s">
+      <c r="P28" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q28" s="55" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1966,22 +1977,22 @@
       <c r="J29" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L29" s="39" t="s">
+      <c r="L29" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="M29" s="50">
+      <c r="M29" s="48">
         <v>34500</v>
       </c>
-      <c r="N29" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O29" s="40">
+      <c r="N29" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="O29" s="48">
         <v>3461</v>
       </c>
-      <c r="P29" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q29" s="44"/>
+      <c r="P29" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q29" s="42"/>
     </row>
     <row r="30" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H30" s="5" t="s">
@@ -1991,69 +2002,69 @@
       <c r="J30" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L30" s="39" t="s">
+      <c r="L30" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="M30" s="50">
+      <c r="M30" s="48">
         <v>21250</v>
       </c>
-      <c r="N30" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O30" s="40">
+      <c r="N30" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="O30" s="48">
         <v>21889</v>
       </c>
-      <c r="P30" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q30" s="44"/>
+      <c r="P30" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q30" s="42"/>
     </row>
     <row r="31" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H31" s="5"/>
       <c r="I31" s="1"/>
       <c r="J31" s="6"/>
-      <c r="L31" s="39" t="s">
+      <c r="L31" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="M31" s="50">
+      <c r="M31" s="48">
         <v>44000</v>
       </c>
-      <c r="N31" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O31" s="40">
+      <c r="N31" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="O31" s="48">
         <v>43996</v>
       </c>
-      <c r="P31" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q31" s="44"/>
+      <c r="P31" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q31" s="42"/>
     </row>
     <row r="32" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H32" s="5" t="s">
         <v>7</v>
       </c>
       <c r="I32" s="1">
-        <f>SUM(I3:I29)</f>
+        <f>SUM(I3:I30)</f>
         <v>0</v>
       </c>
       <c r="J32" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L32" s="53" t="s">
+      <c r="L32" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="M32" s="54"/>
-      <c r="N32" s="55" t="s">
-        <v>3</v>
-      </c>
-      <c r="O32" s="56">
+      <c r="M32" s="52"/>
+      <c r="N32" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="O32" s="52">
         <v>3583</v>
       </c>
-      <c r="P32" s="57" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q32" s="58" t="s">
+      <c r="P32" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q32" s="55" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2068,74 +2079,74 @@
       <c r="J33" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="L33" s="53" t="s">
+      <c r="L33" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="M33" s="54"/>
-      <c r="N33" s="55" t="s">
-        <v>3</v>
-      </c>
-      <c r="O33" s="56">
+      <c r="M33" s="52"/>
+      <c r="N33" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="O33" s="52">
         <v>643</v>
       </c>
-      <c r="P33" s="57" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q33" s="58" t="s">
+      <c r="P33" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q33" s="55" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="34" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="L34" s="53" t="s">
+      <c r="L34" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="M34" s="54"/>
-      <c r="N34" s="55" t="s">
-        <v>3</v>
-      </c>
-      <c r="O34" s="56">
+      <c r="M34" s="52"/>
+      <c r="N34" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="O34" s="52">
         <v>369</v>
       </c>
-      <c r="P34" s="57" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q34" s="58" t="s">
+      <c r="P34" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q34" s="55" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="35" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="L35" s="53" t="s">
+      <c r="L35" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="M35" s="54"/>
-      <c r="N35" s="55" t="s">
-        <v>3</v>
-      </c>
-      <c r="O35" s="56">
+      <c r="M35" s="52"/>
+      <c r="N35" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="O35" s="52">
         <v>446</v>
       </c>
-      <c r="P35" s="57" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q35" s="58" t="s">
+      <c r="P35" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q35" s="55" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="36" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="L36" s="39" t="s">
+      <c r="L36" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="M36" s="50"/>
-      <c r="N36" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O36" s="40">
+      <c r="M36" s="48"/>
+      <c r="N36" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="O36" s="48">
         <v>49749</v>
       </c>
-      <c r="P36" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q36" s="44" t="s">
+      <c r="P36" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q36" s="42" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2146,15 +2157,15 @@
       <c r="L37" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="M37" s="51"/>
-      <c r="N37" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="O37" s="34"/>
-      <c r="P37" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q37" s="37" t="s">
+      <c r="M37" s="49"/>
+      <c r="N37" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="O37" s="49"/>
+      <c r="P37" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q37" s="36" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2173,20 +2184,20 @@
         <v>87</v>
       </c>
       <c r="I38" s="21"/>
-      <c r="L38" s="53" t="s">
+      <c r="L38" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="M38" s="54"/>
-      <c r="N38" s="55" t="s">
-        <v>3</v>
-      </c>
-      <c r="O38" s="56">
+      <c r="M38" s="52"/>
+      <c r="N38" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="O38" s="52">
         <v>6852</v>
       </c>
-      <c r="P38" s="57" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q38" s="58" t="s">
+      <c r="P38" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q38" s="55" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2205,20 +2216,20 @@
         <v>88</v>
       </c>
       <c r="I39" s="17"/>
-      <c r="L39" s="39" t="s">
+      <c r="L39" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="M39" s="50"/>
-      <c r="N39" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O39" s="40">
+      <c r="M39" s="48"/>
+      <c r="N39" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="O39" s="48">
         <v>7532</v>
       </c>
-      <c r="P39" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q39" s="44"/>
+      <c r="P39" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q39" s="42"/>
     </row>
     <row r="40" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D40" s="22" t="s">
@@ -2235,26 +2246,26 @@
         <v>89</v>
       </c>
       <c r="I40" s="24"/>
-      <c r="L40" s="39" t="s">
+      <c r="L40" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="M40" s="50">
+      <c r="M40" s="48">
         <v>236250</v>
       </c>
-      <c r="N40" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O40" s="40">
+      <c r="N40" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="O40" s="48">
         <v>236466</v>
       </c>
-      <c r="P40" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q40" s="44"/>
+      <c r="P40" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q40" s="42"/>
     </row>
     <row r="41" spans="4:17" x14ac:dyDescent="0.25">
       <c r="L41" s="5"/>
-      <c r="M41" s="52"/>
+      <c r="M41" s="50"/>
       <c r="N41" s="1" t="s">
         <v>3</v>
       </c>
@@ -2266,7 +2277,7 @@
     </row>
     <row r="42" spans="4:17" x14ac:dyDescent="0.25">
       <c r="L42" s="5"/>
-      <c r="M42" s="47"/>
+      <c r="M42" s="45"/>
       <c r="N42" s="1" t="s">
         <v>3</v>
       </c>
@@ -2278,7 +2289,7 @@
     </row>
     <row r="43" spans="4:17" x14ac:dyDescent="0.25">
       <c r="L43" s="5"/>
-      <c r="M43" s="47"/>
+      <c r="M43" s="45"/>
       <c r="N43" s="1" t="s">
         <v>3</v>
       </c>
@@ -2290,7 +2301,7 @@
     </row>
     <row r="44" spans="4:17" x14ac:dyDescent="0.25">
       <c r="L44" s="5"/>
-      <c r="M44" s="47"/>
+      <c r="M44" s="45"/>
       <c r="N44" s="1" t="s">
         <v>3</v>
       </c>
@@ -2302,7 +2313,7 @@
     </row>
     <row r="45" spans="4:17" x14ac:dyDescent="0.25">
       <c r="L45" s="5"/>
-      <c r="M45" s="47"/>
+      <c r="M45" s="45"/>
       <c r="N45" s="1" t="s">
         <v>3</v>
       </c>
@@ -2314,7 +2325,7 @@
     </row>
     <row r="46" spans="4:17" x14ac:dyDescent="0.25">
       <c r="L46" s="5"/>
-      <c r="M46" s="47"/>
+      <c r="M46" s="45"/>
       <c r="N46" s="1" t="s">
         <v>3</v>
       </c>
@@ -2326,7 +2337,7 @@
     </row>
     <row r="47" spans="4:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L47" s="7"/>
-      <c r="M47" s="49"/>
+      <c r="M47" s="47"/>
       <c r="N47" s="18" t="s">
         <v>3</v>
       </c>
@@ -2340,19 +2351,28 @@
       <c r="L48" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="M48" s="48">
+      <c r="M48" s="46">
         <f>SUM(M3:M47)</f>
         <v>111556962.36289999</v>
       </c>
       <c r="N48" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="O48" s="48">
+      <c r="O48" s="46">
         <f>SUM(O3:O47)</f>
-        <v>599724</v>
+        <v>111667380.73939998</v>
       </c>
       <c r="P48" s="27" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O49" s="58">
+        <f>O48-149000000</f>
+        <v>-37332619.260600016</v>
+      </c>
+      <c r="P49" s="32" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
continent A coastline, islands
</commit_message>
<xml_diff>
--- a/Not Gplates/Land Calcu.xlsx
+++ b/Not Gplates/Land Calcu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Random stuff\WorldBuild\Gplates - Copy\Not Gplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F61B0F-4332-4A91-B3F2-749E50245CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D341E6-24D3-47CB-A1FB-655EB8CE80CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="130">
   <si>
     <t>Name</t>
   </si>
@@ -405,19 +405,25 @@
     <t>ToDo</t>
   </si>
   <si>
-    <t xml:space="preserve">We need more crust </t>
-  </si>
-  <si>
     <t>kellene még</t>
   </si>
   <si>
     <t>Continent Nemo</t>
   </si>
   <si>
-    <t>Felülvizsgálni az ütközéseket</t>
-  </si>
-  <si>
     <t>Use artistic license</t>
+  </si>
+  <si>
+    <t>MORE ISLANDS</t>
+  </si>
+  <si>
+    <t>Islands J10</t>
+  </si>
+  <si>
+    <t>Islands K9</t>
+  </si>
+  <si>
+    <t>Islands T4</t>
   </si>
 </sst>
 </file>
@@ -788,7 +794,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -834,6 +840,7 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -846,7 +853,6 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -855,10 +861,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1140,10 +1148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:V49"/>
+  <dimension ref="B1:V48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1151,29 +1159,49 @@
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.42578125" customWidth="1"/>
     <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6.42578125" customWidth="1"/>
-    <col min="15" max="15" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="70.28515625" customWidth="1"/>
+    <col min="15" max="15" width="34.7109375" customWidth="1"/>
+    <col min="17" max="17" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="11"/>
+      <c r="M1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="16"/>
+      <c r="O1" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="2" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="11"/>
-      <c r="O2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="12" t="s">
-        <v>5</v>
-      </c>
+      <c r="J2" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="K2" s="56">
+        <v>53209414.484099999</v>
+      </c>
+      <c r="L2" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="59">
+        <f>K2</f>
+        <v>53209414.484099999</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="30"/>
       <c r="S2" s="2" t="s">
         <v>122</v>
       </c>
@@ -1191,33 +1219,31 @@
       <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="M3" s="44">
-        <v>54102303.048900001</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O3" s="55">
-        <f>M3</f>
-        <v>54102303.048900001</v>
-      </c>
-      <c r="P3" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q3" s="30"/>
-      <c r="S3" s="5" t="s">
-        <v>126</v>
-      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="K3" s="45">
+        <v>55076575.485200003</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="55">
+        <f t="shared" ref="M3:M4" si="0">K3</f>
+        <v>55076575.485200003</v>
+      </c>
+      <c r="N3" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" s="30"/>
+      <c r="S3" s="5"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="6"/>
@@ -1226,39 +1252,39 @@
       <c r="B4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="43">
+      <c r="C4" s="44">
         <v>1050</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="M4" s="44">
-        <v>55076575.485200003</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O4" s="55">
-        <f t="shared" ref="O4:O5" si="0">M4</f>
-        <v>55076575.485200003</v>
-      </c>
-      <c r="P4" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q4" s="30"/>
-      <c r="S4" s="5" t="s">
-        <v>123</v>
-      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" s="45">
+        <v>1861282.8287999998</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" s="55">
+        <f t="shared" si="0"/>
+        <v>1861282.8287999998</v>
+      </c>
+      <c r="N4" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="O4" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="S4" s="5"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="V4" s="6"/>
@@ -1267,40 +1293,38 @@
       <c r="B5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="43">
+      <c r="C5" s="44">
         <v>100</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="M5" s="44">
-        <v>1861282.8287999998</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O5" s="55">
-        <f t="shared" si="0"/>
-        <v>1861282.8287999998</v>
-      </c>
-      <c r="P5" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q5" s="30" t="s">
-        <v>51</v>
-      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="K5" s="45">
+        <v>21315235.263500001</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M5" s="55">
+        <f>K5</f>
+        <v>21315235.263500001</v>
+      </c>
+      <c r="N5" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="30"/>
       <c r="S5" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
@@ -1310,31 +1334,30 @@
       <c r="B6" s="5"/>
       <c r="C6" s="1"/>
       <c r="D6" s="6"/>
-      <c r="H6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="32"/>
-      <c r="J6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="M6" s="44">
-        <v>21315235.263500001</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O6" s="55">
-        <f>M6</f>
-        <v>21315235.263500001</v>
-      </c>
-      <c r="P6" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q6" s="30"/>
-      <c r="S6" s="5"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="K6" s="49"/>
+      <c r="L6" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="M6" s="49"/>
+      <c r="N6" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="O6" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
       <c r="V6" s="6"/>
@@ -1350,26 +1373,28 @@
       <c r="D7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="32"/>
-      <c r="J7" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L7" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="M7" s="48"/>
-      <c r="N7" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="O7" s="48"/>
-      <c r="P7" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q7" s="57" t="s">
-        <v>95</v>
+      <c r="G7" s="32"/>
+      <c r="H7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7" s="48"/>
+      <c r="L7" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M7" s="48">
+        <v>236</v>
+      </c>
+      <c r="N7" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O7" s="42" t="s">
+        <v>96</v>
       </c>
       <c r="S7" s="5"/>
       <c r="T7" s="1"/>
@@ -1377,29 +1402,29 @@
       <c r="V7" s="6"/>
     </row>
     <row r="8" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="32"/>
-      <c r="J8" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L8" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="M8" s="47"/>
-      <c r="N8" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O8" s="47">
-        <v>236</v>
-      </c>
-      <c r="P8" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q8" s="41" t="s">
-        <v>96</v>
-      </c>
+      <c r="G8" s="32"/>
+      <c r="H8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="K8" s="48">
+        <v>26300</v>
+      </c>
+      <c r="L8" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M8" s="48">
+        <v>26303</v>
+      </c>
+      <c r="N8" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O8" s="42"/>
       <c r="S8" s="5"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
@@ -1416,29 +1441,31 @@
       <c r="D9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="32"/>
-      <c r="J9" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L9" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="M9" s="47">
-        <v>26300</v>
-      </c>
-      <c r="N9" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O9" s="47">
-        <v>26303</v>
-      </c>
-      <c r="P9" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q9" s="41"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="K9" s="48">
+        <v>1</v>
+      </c>
+      <c r="L9" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M9" s="48">
+        <v>882</v>
+      </c>
+      <c r="N9" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O9" s="42" t="s">
+        <v>97</v>
+      </c>
       <c r="S9" s="5"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
@@ -1449,36 +1476,34 @@
         <v>42</v>
       </c>
       <c r="C10" s="29">
-        <f>O48</f>
-        <v>132992129.76169997</v>
+        <f>M47</f>
+        <v>132457596.99369998</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="F10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="32"/>
-      <c r="J10" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L10" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="M10" s="47">
-        <v>1</v>
-      </c>
-      <c r="N10" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O10" s="47">
-        <v>882</v>
-      </c>
-      <c r="P10" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q10" s="41" t="s">
-        <v>97</v>
+      <c r="G10" s="32"/>
+      <c r="H10" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="K10" s="48"/>
+      <c r="L10" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M10" s="48">
+        <v>363</v>
+      </c>
+      <c r="N10" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O10" s="42" t="s">
+        <v>98</v>
       </c>
       <c r="S10" s="7"/>
       <c r="T10" s="8"/>
@@ -1491,34 +1516,34 @@
       </c>
       <c r="C11" s="29">
         <f>C9-C10</f>
-        <v>377072342.14808828</v>
+        <v>377606874.91608828</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="32"/>
-      <c r="J11" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L11" s="38" t="s">
-        <v>90</v>
-      </c>
-      <c r="M11" s="47"/>
-      <c r="N11" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O11" s="47">
-        <v>363</v>
-      </c>
-      <c r="P11" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q11" s="41" t="s">
-        <v>98</v>
-      </c>
+      <c r="G11" s="32"/>
+      <c r="H11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" s="48">
+        <v>37000</v>
+      </c>
+      <c r="L11" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M11" s="48">
+        <v>38717</v>
+      </c>
+      <c r="N11" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O11" s="42"/>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
@@ -1526,34 +1551,32 @@
       </c>
       <c r="C12" s="1">
         <f>C10*100/C9</f>
-        <v>26.073592082143964</v>
+        <v>25.968794983455915</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="F12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="32"/>
-      <c r="J12" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L12" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="M12" s="47">
-        <v>37000</v>
-      </c>
-      <c r="N12" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O12" s="47">
-        <v>38717</v>
-      </c>
-      <c r="P12" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q12" s="41"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J12" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="K12" s="48"/>
+      <c r="L12" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M12" s="48">
+        <v>816</v>
+      </c>
+      <c r="N12" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O12" s="42"/>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
@@ -1561,32 +1584,34 @@
       </c>
       <c r="C13" s="29">
         <f>C11*100/C9</f>
-        <v>73.926407917856039</v>
+        <v>74.031205016544092</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="32"/>
-      <c r="J13" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L13" s="38" t="s">
-        <v>115</v>
-      </c>
-      <c r="M13" s="47"/>
-      <c r="N13" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O13" s="47">
-        <v>816</v>
-      </c>
-      <c r="P13" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q13" s="41"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J13" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="K13" s="48"/>
+      <c r="L13" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M13" s="48">
+        <v>17074</v>
+      </c>
+      <c r="N13" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O13" s="42" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
@@ -1598,29 +1623,27 @@
       <c r="D14" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="F14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="32"/>
-      <c r="J14" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L14" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="M14" s="47"/>
-      <c r="N14" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O14" s="47">
-        <v>17074</v>
-      </c>
-      <c r="P14" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q14" s="41" t="s">
-        <v>99</v>
-      </c>
+      <c r="G14" s="32"/>
+      <c r="H14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J14" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="K14" s="48"/>
+      <c r="L14" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M14" s="48">
+        <v>1516</v>
+      </c>
+      <c r="N14" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O14" s="42"/>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
@@ -1632,27 +1655,27 @@
       <c r="D15" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="F15" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I15" s="32"/>
-      <c r="J15" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L15" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="M15" s="47"/>
-      <c r="N15" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O15" s="47">
-        <v>1516</v>
-      </c>
-      <c r="P15" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q15" s="41"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J15" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="K15" s="49"/>
+      <c r="L15" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="M15" s="49"/>
+      <c r="N15" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="O15" s="36" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="16" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
@@ -1660,729 +1683,725 @@
       </c>
       <c r="C16" s="8">
         <f>C12-C14</f>
-        <v>-2.9264079178560358</v>
+        <v>-3.0312050165440851</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="F16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="32"/>
-      <c r="J16" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L16" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="M16" s="48"/>
-      <c r="N16" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="O16" s="48"/>
-      <c r="P16" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q16" s="36" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="8:17" x14ac:dyDescent="0.25">
-      <c r="H17" s="5" t="s">
+      <c r="G16" s="32"/>
+      <c r="H16" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="K16" s="49"/>
+      <c r="L16" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="M16" s="49"/>
+      <c r="N16" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="O16" s="36" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F17" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I17" s="32"/>
-      <c r="J17" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L17" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="M17" s="48"/>
-      <c r="N17" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="O17" s="48"/>
-      <c r="P17" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q17" s="36" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="18" spans="8:17" x14ac:dyDescent="0.25">
-      <c r="H18" s="5" t="s">
+      <c r="G17" s="32"/>
+      <c r="H17" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J17" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="K17" s="48"/>
+      <c r="L17" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M17" s="48">
+        <v>22359.376500000002</v>
+      </c>
+      <c r="N17" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O17" s="42" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I18" s="32"/>
-      <c r="J18" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L18" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="M18" s="47"/>
-      <c r="N18" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O18" s="47">
-        <v>22359.376500000002</v>
-      </c>
-      <c r="P18" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q18" s="41" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="8:17" x14ac:dyDescent="0.25">
-      <c r="H19" s="5" t="s">
+      <c r="G18" s="32"/>
+      <c r="H18" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J18" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="K18" s="48"/>
+      <c r="L18" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M18" s="48">
+        <v>34301.792199999996</v>
+      </c>
+      <c r="N18" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O18" s="42" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F19" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I19" s="32"/>
-      <c r="J19" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L19" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="M19" s="47"/>
-      <c r="N19" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O19" s="47">
-        <v>34301.792199999996</v>
-      </c>
-      <c r="P19" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q19" s="41" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" spans="8:17" x14ac:dyDescent="0.25">
-      <c r="H20" s="5" t="s">
+      <c r="G19" s="32"/>
+      <c r="H19" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J19" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="K19" s="48">
+        <v>34000</v>
+      </c>
+      <c r="L19" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M19" s="48">
+        <v>34074</v>
+      </c>
+      <c r="N19" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O19" s="42"/>
+    </row>
+    <row r="20" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F20" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="32"/>
-      <c r="J20" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L20" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="M20" s="47">
-        <v>34000</v>
-      </c>
-      <c r="N20" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O20" s="47">
-        <v>34074</v>
-      </c>
-      <c r="P20" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q20" s="41"/>
-    </row>
-    <row r="21" spans="8:17" x14ac:dyDescent="0.25">
-      <c r="H21" s="5" t="s">
+      <c r="G20" s="32"/>
+      <c r="H20" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J20" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="K20" s="48"/>
+      <c r="L20" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M20" s="48">
+        <v>26071.566500000001</v>
+      </c>
+      <c r="N20" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O20" s="42" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F21" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I21" s="32"/>
-      <c r="J21" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L21" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="M21" s="47"/>
-      <c r="N21" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O21" s="47">
-        <v>26071.566500000001</v>
-      </c>
-      <c r="P21" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q21" s="41" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="22" spans="8:17" x14ac:dyDescent="0.25">
-      <c r="H22" s="5" t="s">
+      <c r="G21" s="32"/>
+      <c r="H21" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J21" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="K21" s="48"/>
+      <c r="L21" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M21" s="48">
+        <v>2307</v>
+      </c>
+      <c r="N21" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O21" s="42" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F22" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I22" s="32"/>
-      <c r="J22" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L22" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="M22" s="47"/>
-      <c r="N22" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O22" s="47">
-        <v>2307</v>
-      </c>
-      <c r="P22" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q22" s="41" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="8:17" x14ac:dyDescent="0.25">
-      <c r="H23" s="5" t="s">
+      <c r="G22" s="32"/>
+      <c r="H22" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J22" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="K22" s="48">
+        <v>71250</v>
+      </c>
+      <c r="L22" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M22" s="48">
+        <v>71285</v>
+      </c>
+      <c r="N22" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O22" s="42"/>
+    </row>
+    <row r="23" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F23" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I23" s="32"/>
-      <c r="J23" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L23" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="M23" s="47">
-        <v>71250</v>
-      </c>
-      <c r="N23" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O23" s="47">
-        <v>71285</v>
-      </c>
-      <c r="P23" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q23" s="41"/>
-    </row>
-    <row r="24" spans="8:17" x14ac:dyDescent="0.25">
-      <c r="H24" s="5" t="s">
+      <c r="G23" s="32"/>
+      <c r="H23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J23" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="K23" s="48"/>
+      <c r="L23" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M23" s="48">
+        <v>18181.400099999995</v>
+      </c>
+      <c r="N23" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O23" s="42" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F24" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I24" s="32"/>
-      <c r="J24" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L24" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="M24" s="47"/>
-      <c r="N24" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O24" s="47">
-        <v>18181.400099999995</v>
-      </c>
-      <c r="P24" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q24" s="41" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="8:17" x14ac:dyDescent="0.25">
-      <c r="H25" s="5" t="s">
+      <c r="G24" s="32"/>
+      <c r="H24" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J24" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="K24" s="49"/>
+      <c r="L24" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="M24" s="49"/>
+      <c r="N24" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="O24" s="36" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F25" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I25" s="32"/>
-      <c r="J25" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L25" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="M25" s="48"/>
-      <c r="N25" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="O25" s="48"/>
-      <c r="P25" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q25" s="36" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="26" spans="8:17" x14ac:dyDescent="0.25">
-      <c r="H26" s="5" t="s">
+      <c r="G25" s="32"/>
+      <c r="H25" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J25" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="K25" s="48">
+        <v>12250</v>
+      </c>
+      <c r="L25" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M25" s="48">
+        <v>13077</v>
+      </c>
+      <c r="N25" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O25" s="42"/>
+    </row>
+    <row r="26" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F26" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I26" s="32"/>
-      <c r="J26" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L26" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="M26" s="47">
-        <v>12250</v>
-      </c>
-      <c r="N26" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O26" s="47">
-        <v>13077</v>
-      </c>
-      <c r="P26" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q26" s="41"/>
-    </row>
-    <row r="27" spans="8:17" x14ac:dyDescent="0.25">
-      <c r="H27" s="5" t="s">
+      <c r="G26" s="32"/>
+      <c r="H26" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J26" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="K26" s="48"/>
+      <c r="L26" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M26" s="48">
+        <v>2402</v>
+      </c>
+      <c r="N26" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O26" s="42"/>
+    </row>
+    <row r="27" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F27" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I27" s="32"/>
-      <c r="J27" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L27" s="38" t="s">
-        <v>71</v>
-      </c>
-      <c r="M27" s="47"/>
-      <c r="N27" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O27" s="47">
-        <v>2402</v>
-      </c>
-      <c r="P27" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q27" s="41"/>
-    </row>
-    <row r="28" spans="8:17" x14ac:dyDescent="0.25">
-      <c r="H28" s="5" t="s">
+      <c r="G27" s="32"/>
+      <c r="H27" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J27" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="K27" s="48"/>
+      <c r="L27" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M27" s="48">
+        <v>1530</v>
+      </c>
+      <c r="N27" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O27" s="42" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F28" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="I28" s="32"/>
-      <c r="J28" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L28" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="M28" s="47"/>
-      <c r="N28" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O28" s="47">
-        <v>1530</v>
-      </c>
-      <c r="P28" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q28" s="41" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="8:17" x14ac:dyDescent="0.25">
-      <c r="H29" s="5" t="s">
+      <c r="G28" s="32"/>
+      <c r="H28" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J28" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="K28" s="48">
+        <v>34500</v>
+      </c>
+      <c r="L28" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M28" s="48">
+        <v>3461</v>
+      </c>
+      <c r="N28" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O28" s="42"/>
+    </row>
+    <row r="29" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F29" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="I29" s="32"/>
-      <c r="J29" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L29" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="M29" s="47">
-        <v>34500</v>
-      </c>
-      <c r="N29" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O29" s="47">
-        <v>3461</v>
-      </c>
-      <c r="P29" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q29" s="41"/>
-    </row>
-    <row r="30" spans="8:17" x14ac:dyDescent="0.25">
-      <c r="H30" s="5" t="s">
+      <c r="G29" s="32"/>
+      <c r="H29" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J29" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="K29" s="48">
+        <v>21250</v>
+      </c>
+      <c r="L29" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M29" s="48">
+        <v>21889</v>
+      </c>
+      <c r="N29" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O29" s="42"/>
+    </row>
+    <row r="30" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F30" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="I30" s="1"/>
-      <c r="J30" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L30" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="M30" s="47">
-        <v>21250</v>
-      </c>
-      <c r="N30" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O30" s="47">
-        <v>21889</v>
-      </c>
-      <c r="P30" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q30" s="41"/>
-    </row>
-    <row r="31" spans="8:17" x14ac:dyDescent="0.25">
-      <c r="H31" s="5"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="6"/>
-      <c r="L31" s="38" t="s">
+      <c r="G30" s="1"/>
+      <c r="H30" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J30" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="M31" s="47">
+      <c r="K30" s="48">
         <v>44000</v>
       </c>
-      <c r="N31" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O31" s="47">
+      <c r="L30" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M30" s="48">
         <v>43996</v>
       </c>
-      <c r="P31" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q31" s="41"/>
-    </row>
-    <row r="32" spans="8:17" x14ac:dyDescent="0.25">
-      <c r="H32" s="5" t="s">
+      <c r="N30" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O30" s="42"/>
+    </row>
+    <row r="31" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F31" s="5"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="6"/>
+      <c r="J31" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="K31" s="48"/>
+      <c r="L31" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M31" s="48">
+        <v>3583</v>
+      </c>
+      <c r="N31" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O31" s="42" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F32" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I32" s="1">
-        <f>SUM(I3:I30)</f>
+      <c r="G32" s="1">
+        <f>SUM(G3:G30)</f>
         <v>0</v>
       </c>
-      <c r="J32" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L32" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="M32" s="47"/>
-      <c r="N32" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O32" s="47">
-        <v>3583</v>
-      </c>
-      <c r="P32" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q32" s="41" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="33" spans="4:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H33" s="7" t="s">
+      <c r="H32" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J32" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="K32" s="48"/>
+      <c r="L32" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M32" s="48">
+        <v>643</v>
+      </c>
+      <c r="N32" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O32" s="42" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F33" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I33" s="8">
-        <f>I34-I32</f>
+      <c r="G33" s="8">
+        <f>I34-G32</f>
         <v>0</v>
       </c>
-      <c r="J33" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L33" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="M33" s="47"/>
-      <c r="N33" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O33" s="47">
-        <v>643</v>
-      </c>
-      <c r="P33" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q33" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="34" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="L34" s="38" t="s">
+      <c r="H33" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J33" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="M34" s="47"/>
-      <c r="N34" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O34" s="47">
+      <c r="K33" s="48"/>
+      <c r="L33" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M33" s="48">
         <v>369</v>
       </c>
-      <c r="P34" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q34" s="41" t="s">
+      <c r="N33" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O33" s="42" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="35" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="L35" s="38" t="s">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J34" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="M35" s="47"/>
-      <c r="N35" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O35" s="47">
+      <c r="K34" s="48"/>
+      <c r="L34" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M34" s="48">
         <v>446</v>
       </c>
-      <c r="P35" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q35" s="41" t="s">
+      <c r="N34" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O34" s="42" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="36" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="L36" s="33" t="s">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J35" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="M36" s="48"/>
-      <c r="N36" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="O36" s="48"/>
-      <c r="P36" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q36" s="36" t="s">
+      <c r="K35" s="49"/>
+      <c r="L35" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="M35" s="49"/>
+      <c r="N35" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="O35" s="36" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D37" t="s">
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J36" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="K36" s="49"/>
+      <c r="L36" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="M36" s="49"/>
+      <c r="N36" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="O36" s="36" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>6</v>
       </c>
-      <c r="L37" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="M37" s="48"/>
-      <c r="N37" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="O37" s="48"/>
-      <c r="P37" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q37" s="36" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="38" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D38" s="19" t="s">
+      <c r="J37" s="50" t="s">
+        <v>114</v>
+      </c>
+      <c r="K37" s="51"/>
+      <c r="L37" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="M37" s="51">
+        <v>6852</v>
+      </c>
+      <c r="N37" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="O37" s="54" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B38" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E38" s="19" t="s">
+      <c r="C38" s="19" t="s">
         <v>81</v>
       </c>
+      <c r="D38" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E38" s="20"/>
       <c r="F38" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="I38" s="21"/>
-      <c r="L38" s="50" t="s">
-        <v>114</v>
-      </c>
-      <c r="M38" s="51"/>
-      <c r="N38" s="52" t="s">
-        <v>3</v>
-      </c>
-      <c r="O38" s="51">
-        <v>6852</v>
-      </c>
-      <c r="P38" s="53" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q38" s="54" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="39" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D39" s="14" t="s">
+      <c r="G38" s="21"/>
+      <c r="J38" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="K38" s="48"/>
+      <c r="L38" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M38" s="48">
+        <v>7532</v>
+      </c>
+      <c r="N38" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O38" s="42"/>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B39" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="E39" s="14" t="s">
+      <c r="C39" s="14" t="s">
         <v>82</v>
       </c>
+      <c r="D39" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E39" s="1"/>
       <c r="F39" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="I39" s="17"/>
-      <c r="L39" s="38" t="s">
-        <v>117</v>
-      </c>
-      <c r="M39" s="47"/>
-      <c r="N39" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O39" s="47">
-        <v>7532</v>
-      </c>
-      <c r="P39" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q39" s="41"/>
-    </row>
-    <row r="40" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D40" s="22" t="s">
+      <c r="G39" s="17"/>
+      <c r="J39" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="K39" s="48">
+        <v>236250</v>
+      </c>
+      <c r="L39" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M39" s="48">
+        <v>236466</v>
+      </c>
+      <c r="N39" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O39" s="42"/>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B40" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="E40" s="22" t="s">
+      <c r="C40" s="22" t="s">
         <v>83</v>
       </c>
+      <c r="D40" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E40" s="23"/>
       <c r="F40" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="G40" s="23"/>
-      <c r="H40" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="I40" s="24"/>
-      <c r="L40" s="38" t="s">
-        <v>118</v>
-      </c>
-      <c r="M40" s="47">
-        <v>236250</v>
-      </c>
-      <c r="N40" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O40" s="47">
-        <v>236466</v>
-      </c>
-      <c r="P40" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q40" s="41"/>
-    </row>
-    <row r="41" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="L41" s="5"/>
-      <c r="M41" s="49"/>
-      <c r="N41" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O41" s="14"/>
-      <c r="P41" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q41" s="30"/>
-    </row>
-    <row r="42" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="L42" s="5"/>
-      <c r="M42" s="44"/>
-      <c r="N42" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O42" s="14"/>
-      <c r="P42" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q42" s="30"/>
-    </row>
-    <row r="43" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="L43" s="5"/>
-      <c r="M43" s="44"/>
-      <c r="N43" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O43" s="14"/>
-      <c r="P43" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q43" s="30"/>
-    </row>
-    <row r="44" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="L44" s="5"/>
-      <c r="M44" s="44"/>
-      <c r="N44" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O44" s="14"/>
-      <c r="P44" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q44" s="30"/>
-    </row>
-    <row r="45" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="L45" s="5"/>
-      <c r="M45" s="44"/>
-      <c r="N45" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O45" s="14"/>
-      <c r="P45" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q45" s="30"/>
-    </row>
-    <row r="46" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="L46" s="5"/>
-      <c r="M46" s="44"/>
-      <c r="N46" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O46" s="14"/>
-      <c r="P46" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q46" s="30"/>
-    </row>
-    <row r="47" spans="4:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L47" s="7"/>
-      <c r="M47" s="46"/>
-      <c r="N47" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="O47" s="15"/>
-      <c r="P47" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q47" s="31"/>
-    </row>
-    <row r="48" spans="4:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L48" s="25" t="s">
+      <c r="G40" s="24"/>
+      <c r="J40" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="K40" s="48"/>
+      <c r="L40" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M40" s="39">
+        <v>11618.645199999999</v>
+      </c>
+      <c r="N40" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O40" s="42"/>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J41" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="K41" s="56"/>
+      <c r="L41" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M41" s="39">
+        <v>206762.14379999999</v>
+      </c>
+      <c r="N41" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O41" s="42"/>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J42" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="K42" s="56"/>
+      <c r="L42" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M42" s="39">
+        <v>139975.00779999999</v>
+      </c>
+      <c r="N42" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O42" s="42"/>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J43" s="5"/>
+      <c r="K43" s="45"/>
+      <c r="L43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M43" s="14"/>
+      <c r="N43" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="O43" s="30"/>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J44" s="5"/>
+      <c r="K44" s="45"/>
+      <c r="L44" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M44" s="14"/>
+      <c r="N44" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="O44" s="30"/>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J45" s="5"/>
+      <c r="K45" s="45"/>
+      <c r="L45" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M45" s="14"/>
+      <c r="N45" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="O45" s="30"/>
+    </row>
+    <row r="46" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J46" s="7"/>
+      <c r="K46" s="47"/>
+      <c r="L46" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="M46" s="15"/>
+      <c r="N46" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="O46" s="31"/>
+    </row>
+    <row r="47" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J47" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="M48" s="45">
-        <f>SUM(M3:M47)</f>
-        <v>132872197.62639999</v>
-      </c>
-      <c r="N48" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="O48" s="45">
-        <f>SUM(O3:O47)</f>
-        <v>132992129.76169997</v>
-      </c>
-      <c r="P48" s="27" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="15:16" x14ac:dyDescent="0.25">
-      <c r="O49" s="56">
-        <f>O48-149000000</f>
-        <v>-16007870.238300025</v>
-      </c>
-      <c r="P49" s="32" t="s">
-        <v>124</v>
+      <c r="K47" s="46">
+        <f>SUM(K2:K46)</f>
+        <v>131979309.0616</v>
+      </c>
+      <c r="L47" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="M47" s="46">
+        <f>SUM(M2:M46)</f>
+        <v>132457596.99369998</v>
+      </c>
+      <c r="N47" s="27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="M48" s="57">
+        <f>M47-149000000</f>
+        <v>-16542403.006300017</v>
+      </c>
+      <c r="N48" s="32" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
continent B coast, islands, exit
</commit_message>
<xml_diff>
--- a/Not Gplates/Land Calcu.xlsx
+++ b/Not Gplates/Land Calcu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Random stuff\WorldBuild\Gplates - Copy\Not Gplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D341E6-24D3-47CB-A1FB-655EB8CE80CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F6976F-FEB9-48D2-B3AD-D9A3DDD1CDC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="133">
   <si>
     <t>Name</t>
   </si>
@@ -424,6 +424,15 @@
   </si>
   <si>
     <t>Islands T4</t>
+  </si>
+  <si>
+    <t>Continent A SZ Islands</t>
+  </si>
+  <si>
+    <t>Continent B Sz Island</t>
+  </si>
+  <si>
+    <t>Microcontintent</t>
   </si>
 </sst>
 </file>
@@ -1151,7 +1160,7 @@
   <dimension ref="B1:V48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,18 +1235,17 @@
       <c r="H3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="K3" s="45">
+      <c r="K3" s="56">
         <v>55076575.485200003</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M3" s="55">
-        <f t="shared" ref="M3:M4" si="0">K3</f>
-        <v>55076575.485200003</v>
+      <c r="L3" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="59">
+        <v>55094497.448899999</v>
       </c>
       <c r="N3" s="17" t="s">
         <v>3</v>
@@ -1275,7 +1283,7 @@
         <v>3</v>
       </c>
       <c r="M4" s="55">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="M3:M4" si="0">K4</f>
         <v>1861282.8287999998</v>
       </c>
       <c r="N4" s="17" t="s">
@@ -1284,7 +1292,9 @@
       <c r="O4" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="S4" s="5"/>
+      <c r="S4" s="5" t="s">
+        <v>132</v>
+      </c>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="V4" s="6"/>
@@ -1477,7 +1487,7 @@
       </c>
       <c r="C10" s="29">
         <f>M47</f>
-        <v>132457596.99369998</v>
+        <v>132631950.37509999</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>3</v>
@@ -1516,7 +1526,7 @@
       </c>
       <c r="C11" s="29">
         <f>C9-C10</f>
-        <v>377606874.91608828</v>
+        <v>377432521.53468823</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>3</v>
@@ -1551,7 +1561,7 @@
       </c>
       <c r="C12" s="1">
         <f>C10*100/C9</f>
-        <v>25.968794983455915</v>
+        <v>26.002977599772471</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>49</v>
@@ -1584,7 +1594,7 @@
       </c>
       <c r="C13" s="29">
         <f>C11*100/C9</f>
-        <v>74.031205016544092</v>
+        <v>73.997022400227522</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>49</v>
@@ -1683,7 +1693,7 @@
       </c>
       <c r="C16" s="8">
         <f>C12-C14</f>
-        <v>-3.0312050165440851</v>
+        <v>-2.9970224002275287</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>49</v>
@@ -2259,7 +2269,7 @@
         <v>3</v>
       </c>
       <c r="M39" s="48">
-        <v>236466</v>
+        <v>334338.82849999995</v>
       </c>
       <c r="N39" s="41" t="s">
         <v>3</v>
@@ -2329,28 +2339,36 @@
       <c r="O42" s="42"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="J43" s="5"/>
-      <c r="K43" s="45"/>
-      <c r="L43" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M43" s="14"/>
-      <c r="N43" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="O43" s="30"/>
+      <c r="J43" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="K43" s="56"/>
+      <c r="L43" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M43" s="39">
+        <v>27742.253799999999</v>
+      </c>
+      <c r="N43" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O43" s="42"/>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="J44" s="5"/>
-      <c r="K44" s="45"/>
-      <c r="L44" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M44" s="14"/>
-      <c r="N44" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="O44" s="30"/>
+      <c r="J44" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="K44" s="56"/>
+      <c r="L44" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="M44" s="39">
+        <v>30816.3354</v>
+      </c>
+      <c r="N44" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O44" s="42"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="J45" s="5"/>
@@ -2389,7 +2407,7 @@
       </c>
       <c r="M47" s="46">
         <f>SUM(M2:M46)</f>
-        <v>132457596.99369998</v>
+        <v>132631950.37509999</v>
       </c>
       <c r="N47" s="27" t="s">
         <v>3</v>
@@ -2398,7 +2416,7 @@
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="M48" s="57">
         <f>M47-149000000</f>
-        <v>-16542403.006300017</v>
+        <v>-16368049.624900013</v>
       </c>
       <c r="N48" s="32" t="s">
         <v>123</v>

</xml_diff>